<commit_message>
Commit by Sneha(2nd commit)
</commit_message>
<xml_diff>
--- a/Excelerate/src/test/resources/testcase.xlsx
+++ b/Excelerate/src/test/resources/testcase.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclippse\Excelerate\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91630\git\repository\Excelerate\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891B9713-0686-4AA8-96A4-E22A1C8573FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1D5332-EED0-42AC-89AD-64B30E92FD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>http://automationexercise.com</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>B@bumisuni5143</t>
+  </si>
+  <si>
+    <t>D@sneha123</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1121,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1158,7 +1161,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
commit By Sneha(4th commit)
</commit_message>
<xml_diff>
--- a/Excelerate/src/test/resources/testcase.xlsx
+++ b/Excelerate/src/test/resources/testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91630\git\repository\Excelerate\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1D5332-EED0-42AC-89AD-64B30E92FD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C9D1B0-735E-4952-A77A-2BB0E70A48EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t>http://automationexercise.com</t>
   </si>
@@ -155,12 +155,6 @@
     <t>siddela</t>
   </si>
   <si>
-    <t>snehasiddela11@gmail.com</t>
-  </si>
-  <si>
-    <t>S@sneha123</t>
-  </si>
-  <si>
     <t>padmu</t>
   </si>
   <si>
@@ -170,9 +164,6 @@
     <t>padmusham@gmail.com</t>
   </si>
   <si>
-    <t>P@padmu123</t>
-  </si>
-  <si>
     <t>P@padmu</t>
   </si>
   <si>
@@ -188,7 +179,16 @@
     <t>B@bumisuni5143</t>
   </si>
   <si>
-    <t>D@sneha123</t>
+    <t>S@sneha1234</t>
+  </si>
+  <si>
+    <t>P@padmu12345</t>
+  </si>
+  <si>
+    <t>snehasiddela175@gmail.com</t>
+  </si>
+  <si>
+    <t>S@sneha789</t>
   </si>
 </sst>
 </file>
@@ -1118,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CFEB7DC-0D3D-4662-8B47-EA85D68A776A}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1158,60 +1158,72 @@
         <v>39</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="D3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="E4" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>50</v>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="D6" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{1D7BDF73-4AE6-491F-8789-3CCA7DE6D31A}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{71CAAC2F-800D-42F3-BBE7-5FC521E028B2}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{B6E1FE73-DFDB-4ED5-AAEA-C639DFF26316}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{8346707F-8276-4B2B-9A0C-C0D22DA5A92A}"/>
-    <hyperlink ref="D3" r:id="rId5" xr:uid="{F4C8DE45-0D68-478D-98AB-4F6015ABEDBA}"/>
-    <hyperlink ref="E3" r:id="rId6" xr:uid="{E20AE72B-6B7A-4BCB-93C9-22733550426B}"/>
-    <hyperlink ref="C4" r:id="rId7" xr:uid="{834AE574-9A4E-4F97-889E-A86279A89F87}"/>
-    <hyperlink ref="D4" r:id="rId8" xr:uid="{D1F14185-8FEF-4ACC-B038-D94B2FA1CB18}"/>
-    <hyperlink ref="E4" r:id="rId9" xr:uid="{4DD3FF23-53A9-4817-AA97-89F31684A151}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{8346707F-8276-4B2B-9A0C-C0D22DA5A92A}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{F4C8DE45-0D68-478D-98AB-4F6015ABEDBA}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{E20AE72B-6B7A-4BCB-93C9-22733550426B}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{834AE574-9A4E-4F97-889E-A86279A89F87}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{D1F14185-8FEF-4ACC-B038-D94B2FA1CB18}"/>
+    <hyperlink ref="E4" r:id="rId7" xr:uid="{4DD3FF23-53A9-4817-AA97-89F31684A151}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{1752B806-B5CF-4FCF-AEC1-A97706B320FF}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{FDA6E0F1-7976-4FEE-9762-60C641B68810}"/>
+    <hyperlink ref="D2" r:id="rId10" xr:uid="{B9794339-F43A-4AD5-85B4-B0C4E11AB321}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>